<commit_message>
all data points captured
</commit_message>
<xml_diff>
--- a/NFES_Review/_jupyterPlots/deltaErrors.xlsx
+++ b/NFES_Review/_jupyterPlots/deltaErrors.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oskat\OneDrive - Instituto Tecnologico y de Estudios Superiores de Monterrey\Documents\MNT_ITESM_Thesis\NFES_Review\_jupyterPlots\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83A5D8A6-77D5-4408-9E85-BE2CFD80C2D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69F5B9D4-D0F4-4037-A6C6-3F515CB6C806}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1170" yWindow="1170" windowWidth="12135" windowHeight="11385" xr2:uid="{DA9E80A8-F6DD-45B3-A7FC-79AA849154BA}"/>
   </bookViews>
@@ -445,8 +445,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA9B74E9-4996-4CE6-B1B8-5F6373B355B6}">
   <dimension ref="A1:E143"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A128" workbookViewId="0">
-      <selection activeCell="F142" sqref="F142"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="G51" sqref="G51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -455,7 +455,7 @@
     <col min="2" max="2" width="24.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="2"/>
+    <col min="5" max="5" width="6.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
plots with no axis breaks
</commit_message>
<xml_diff>
--- a/NFES_Review/_jupyterPlots/deltaErrors.xlsx
+++ b/NFES_Review/_jupyterPlots/deltaErrors.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oskat\OneDrive - Instituto Tecnologico y de Estudios Superiores de Monterrey\Documents\MNT_ITESM_Thesis\NFES_Review\_jupyterPlots\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69F5B9D4-D0F4-4037-A6C6-3F515CB6C806}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0E0450A-8DE7-4DAF-85F7-B34D93ADDB6F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1170" yWindow="1170" windowWidth="12135" windowHeight="11385" xr2:uid="{DA9E80A8-F6DD-45B3-A7FC-79AA849154BA}"/>
   </bookViews>
@@ -445,8 +445,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA9B74E9-4996-4CE6-B1B8-5F6373B355B6}">
   <dimension ref="A1:E143"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="G51" sqref="G51"/>
+    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="E103" sqref="E103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -454,8 +454,8 @@
     <col min="1" max="1" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" style="2" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="9" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -491,7 +491,7 @@
         <v>NAN</v>
       </c>
       <c r="E2" s="2" t="str">
-        <f>IF(ISNUMBER(B2),ABS((C2-B2)/(B2)),"NAN")</f>
+        <f>IF(ISNUMBER(B2),ABS((C2-B2)/(B2))*100,"NAN")</f>
         <v>NAN</v>
       </c>
     </row>
@@ -510,7 +510,7 @@
         <v>NAN</v>
       </c>
       <c r="E3" s="2" t="str">
-        <f t="shared" ref="E3:E66" si="1">IF(ISNUMBER(B3),ABS((C3-B3)/(B3)),"NAN")</f>
+        <f t="shared" ref="E3:E66" si="1">IF(ISNUMBER(B3),ABS((C3-B3)/(B3))*100,"NAN")</f>
         <v>NAN</v>
       </c>
     </row>
@@ -1385,7 +1385,7 @@
       </c>
       <c r="E49" s="2">
         <f t="shared" si="1"/>
-        <v>9.4138738738738734</v>
+        <v>941.38738738738732</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -1404,7 +1404,7 @@
       </c>
       <c r="E50" s="2">
         <f t="shared" si="1"/>
-        <v>8.0469947559499797</v>
+        <v>804.69947559499792</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -1423,7 +1423,7 @@
       </c>
       <c r="E51" s="2">
         <f t="shared" si="1"/>
-        <v>10.795839720317332</v>
+        <v>1079.5839720317331</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -1442,7 +1442,7 @@
       </c>
       <c r="E52" s="2">
         <f t="shared" si="1"/>
-        <v>10.795839720317332</v>
+        <v>1079.5839720317331</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -1461,7 +1461,7 @@
       </c>
       <c r="E53" s="2">
         <f t="shared" si="1"/>
-        <v>8.0469947559499797</v>
+        <v>804.69947559499792</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -1480,7 +1480,7 @@
       </c>
       <c r="E54" s="2">
         <f t="shared" si="1"/>
-        <v>9.4138738738738734</v>
+        <v>941.38738738738732</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -1499,7 +1499,7 @@
       </c>
       <c r="E55" s="2">
         <f t="shared" si="1"/>
-        <v>8.0469947559499797</v>
+        <v>804.69947559499792</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
@@ -1518,7 +1518,7 @@
       </c>
       <c r="E56" s="2">
         <f t="shared" si="1"/>
-        <v>9.4138738738738734</v>
+        <v>941.38738738738732</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -1537,7 +1537,7 @@
       </c>
       <c r="E57" s="2">
         <f t="shared" si="1"/>
-        <v>9.4138738738738734</v>
+        <v>941.38738738738732</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -1556,7 +1556,7 @@
       </c>
       <c r="E58" s="2">
         <f t="shared" si="1"/>
-        <v>8.0469947559499797</v>
+        <v>804.69947559499792</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -1575,7 +1575,7 @@
       </c>
       <c r="E59" s="2">
         <f t="shared" si="1"/>
-        <v>9.4138738738738734</v>
+        <v>941.38738738738732</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -1594,7 +1594,7 @@
       </c>
       <c r="E60" s="2">
         <f t="shared" si="1"/>
-        <v>8.0469947559499797</v>
+        <v>804.69947559499792</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -1613,7 +1613,7 @@
       </c>
       <c r="E61" s="2">
         <f t="shared" si="1"/>
-        <v>10.795839720317332</v>
+        <v>1079.5839720317331</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -1632,7 +1632,7 @@
       </c>
       <c r="E62" s="2">
         <f t="shared" si="1"/>
-        <v>9.4138738738738734</v>
+        <v>941.38738738738732</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -1651,7 +1651,7 @@
       </c>
       <c r="E63" s="2">
         <f t="shared" si="1"/>
-        <v>8.0469947559499797</v>
+        <v>804.69947559499792</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
@@ -1670,7 +1670,7 @@
       </c>
       <c r="E64" s="2">
         <f t="shared" si="1"/>
-        <v>8.0469947559499797</v>
+        <v>804.69947559499792</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -1689,7 +1689,7 @@
       </c>
       <c r="E65" s="2">
         <f t="shared" si="1"/>
-        <v>2.830769230769236E-2</v>
+        <v>2.8307692307692358</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
@@ -1708,7 +1708,7 @@
       </c>
       <c r="E66" s="2">
         <f t="shared" si="1"/>
-        <v>0.10846153846153841</v>
+        <v>10.846153846153841</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
@@ -1726,8 +1726,8 @@
         <v>0.40999999999999659</v>
       </c>
       <c r="E67" s="2">
-        <f t="shared" ref="E67:E130" si="3">IF(ISNUMBER(B67),ABS((C67-B67)/(B67)),"NAN")</f>
-        <v>6.3076923076922555E-3</v>
+        <f t="shared" ref="E67:E130" si="3">IF(ISNUMBER(B67),ABS((C67-B67)/(B67))*100,"NAN")</f>
+        <v>0.63076923076922553</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
@@ -1746,7 +1746,7 @@
       </c>
       <c r="E68" s="2">
         <f t="shared" si="3"/>
-        <v>2.7538461538461526E-2</v>
+        <v>2.7538461538461525</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
@@ -1765,7 +1765,7 @@
       </c>
       <c r="E69" s="2">
         <f t="shared" si="3"/>
-        <v>6.8769230769230749E-2</v>
+        <v>6.8769230769230747</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
@@ -1784,7 +1784,7 @@
       </c>
       <c r="E70" s="2">
         <f t="shared" si="3"/>
-        <v>6.8769230769230749E-2</v>
+        <v>6.8769230769230747</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
@@ -1803,7 +1803,7 @@
       </c>
       <c r="E71" s="2">
         <f t="shared" si="3"/>
-        <v>2.9138603332151611E-2</v>
+        <v>2.9138603332151609</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -1822,7 +1822,7 @@
       </c>
       <c r="E72" s="2">
         <f t="shared" si="3"/>
-        <v>2.9138603332151611E-2</v>
+        <v>2.9138603332151609</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
@@ -1841,7 +1841,7 @@
       </c>
       <c r="E73" s="2">
         <f t="shared" si="3"/>
-        <v>4.820985466146744E-2</v>
+        <v>4.8209854661467437</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -1860,7 +1860,7 @@
       </c>
       <c r="E74" s="2">
         <f t="shared" si="3"/>
-        <v>4.9769585253456088E-2</v>
+        <v>4.9769585253456086</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
@@ -1879,7 +1879,7 @@
       </c>
       <c r="E75" s="2">
         <f t="shared" si="3"/>
-        <v>6.7281105990783269E-2</v>
+        <v>6.7281105990783265</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
@@ -1898,7 +1898,7 @@
       </c>
       <c r="E76" s="2">
         <f t="shared" si="3"/>
-        <v>4.8883374689826169E-2</v>
+        <v>4.8883374689826171</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
@@ -1917,7 +1917,7 @@
       </c>
       <c r="E77" s="2">
         <f t="shared" si="3"/>
-        <v>6.5470120334488666E-3</v>
+        <v>0.65470120334488668</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
@@ -1936,7 +1936,7 @@
       </c>
       <c r="E78" s="2">
         <f t="shared" si="3"/>
-        <v>2.612686110544565E-2</v>
+        <v>2.6126861105445651</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
@@ -1955,7 +1955,7 @@
       </c>
       <c r="E79" s="2">
         <f t="shared" si="3"/>
-        <v>1.4929634917397497E-2</v>
+        <v>1.4929634917397496</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
@@ -1974,7 +1974,7 @@
       </c>
       <c r="E80" s="2">
         <f t="shared" si="3"/>
-        <v>1.6092188456047291E-2</v>
+        <v>1.6092188456047292</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
@@ -1993,7 +1993,7 @@
       </c>
       <c r="E81" s="2">
         <f t="shared" si="3"/>
-        <v>3.6324699163777285E-2</v>
+        <v>3.6324699163777288</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
@@ -2012,7 +2012,7 @@
       </c>
       <c r="E82" s="2">
         <f t="shared" si="3"/>
-        <v>5.9147460738323008E-3</v>
+        <v>0.5914746073832301</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
@@ -2031,7 +2031,7 @@
       </c>
       <c r="E83" s="2">
         <f t="shared" si="3"/>
-        <v>5.9147460738323008E-3</v>
+        <v>0.5914746073832301</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
@@ -2050,7 +2050,7 @@
       </c>
       <c r="E84" s="2">
         <f t="shared" si="3"/>
-        <v>2.1384092838947089E-2</v>
+        <v>2.1384092838947089</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
@@ -2069,7 +2069,7 @@
       </c>
       <c r="E85" s="2">
         <f t="shared" si="3"/>
-        <v>2.1270874610812302E-2</v>
+        <v>2.12708746108123</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
@@ -2088,7 +2088,7 @@
       </c>
       <c r="E86" s="2">
         <f t="shared" si="3"/>
-        <v>2.1384092838947089E-2</v>
+        <v>2.1384092838947089</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
@@ -2107,7 +2107,7 @@
       </c>
       <c r="E87" s="2">
         <f t="shared" si="3"/>
-        <v>2.503538069629218E-2</v>
+        <v>2.5035380696292178</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
@@ -2126,7 +2126,7 @@
       </c>
       <c r="E88" s="2">
         <f t="shared" si="3"/>
-        <v>2.8913105009906685E-2</v>
+        <v>2.8913105009906683</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
@@ -2145,7 +2145,7 @@
       </c>
       <c r="E89" s="2">
         <f t="shared" si="3"/>
-        <v>3.5847721483158845E-2</v>
+        <v>3.5847721483158845</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
@@ -2164,7 +2164,7 @@
       </c>
       <c r="E90" s="2">
         <f t="shared" si="3"/>
-        <v>4.3971129351825712E-2</v>
+        <v>4.3971129351825713</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
@@ -2183,7 +2183,7 @@
       </c>
       <c r="E91" s="2">
         <f t="shared" si="3"/>
-        <v>0.13709999999999997</v>
+        <v>13.709999999999997</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
@@ -2202,7 +2202,7 @@
       </c>
       <c r="E92" s="2">
         <f t="shared" si="3"/>
-        <v>0.14853333333333335</v>
+        <v>14.853333333333335</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
@@ -2221,7 +2221,7 @@
       </c>
       <c r="E93" s="2">
         <f t="shared" si="3"/>
-        <v>0.10843333333333324</v>
+        <v>10.843333333333325</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
@@ -2240,7 +2240,7 @@
       </c>
       <c r="E94" s="2">
         <f t="shared" si="3"/>
-        <v>1.113333333333325E-2</v>
+        <v>1.1133333333333251</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
@@ -2259,7 +2259,7 @@
       </c>
       <c r="E95" s="2">
         <f t="shared" si="3"/>
-        <v>0.14439999999999997</v>
+        <v>14.439999999999998</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
@@ -2278,7 +2278,7 @@
       </c>
       <c r="E96" s="2">
         <f t="shared" si="3"/>
-        <v>8.4666666666666585E-2</v>
+        <v>8.4666666666666579</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
@@ -2297,7 +2297,7 @@
       </c>
       <c r="E97" s="2">
         <f t="shared" si="3"/>
-        <v>0.16951520000000003</v>
+        <v>16.951520000000002</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
@@ -2316,7 +2316,7 @@
       </c>
       <c r="E98" s="2">
         <f t="shared" si="3"/>
-        <v>0.17301720000000001</v>
+        <v>17.30172</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
@@ -2335,7 +2335,7 @@
       </c>
       <c r="E99" s="2">
         <f t="shared" si="3"/>
-        <v>0.13422320000000007</v>
+        <v>13.422320000000006</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
@@ -2354,7 +2354,7 @@
       </c>
       <c r="E100" s="2">
         <f t="shared" si="3"/>
-        <v>9.2685200000000037E-2</v>
+        <v>9.2685200000000041</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
@@ -2373,7 +2373,7 @@
       </c>
       <c r="E101" s="2">
         <f t="shared" si="3"/>
-        <v>0.10092</v>
+        <v>10.091999999999999</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
@@ -2392,7 +2392,7 @@
       </c>
       <c r="E102" s="2">
         <f t="shared" si="3"/>
-        <v>8.0570000000000003E-2</v>
+        <v>8.0570000000000004</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
@@ -2411,7 +2411,7 @@
       </c>
       <c r="E103" s="2">
         <f t="shared" si="3"/>
-        <v>0.22859780621572218</v>
+        <v>22.859780621572217</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
@@ -2430,7 +2430,7 @@
       </c>
       <c r="E104" s="2">
         <f t="shared" si="3"/>
-        <v>0.20909323583180983</v>
+        <v>20.909323583180985</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
@@ -2449,7 +2449,7 @@
       </c>
       <c r="E105" s="2">
         <f t="shared" si="3"/>
-        <v>7.749542961608835E-3</v>
+        <v>0.77495429616088352</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
@@ -2468,7 +2468,7 @@
       </c>
       <c r="E106" s="2">
         <f t="shared" si="3"/>
-        <v>4.6906764168190111E-2</v>
+        <v>4.6906764168190112</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
@@ -2487,7 +2487,7 @@
       </c>
       <c r="E107" s="2">
         <f t="shared" si="3"/>
-        <v>0.10682998171846429</v>
+        <v>10.68299817184643</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
@@ -2506,7 +2506,7 @@
       </c>
       <c r="E108" s="2">
         <f t="shared" si="3"/>
-        <v>0.20627970749542968</v>
+        <v>20.627970749542968</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
@@ -2525,7 +2525,7 @@
       </c>
       <c r="E109" s="2">
         <f t="shared" si="3"/>
-        <v>0.21730347349177323</v>
+        <v>21.730347349177322</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
@@ -2544,7 +2544,7 @@
       </c>
       <c r="E110" s="2">
         <f t="shared" si="3"/>
-        <v>0.25701828153564904</v>
+        <v>25.701828153564904</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
@@ -2563,7 +2563,7 @@
       </c>
       <c r="E111" s="2">
         <f t="shared" si="3"/>
-        <v>0.37800182815356492</v>
+        <v>37.800182815356493</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
@@ -2582,7 +2582,7 @@
       </c>
       <c r="E112" s="2">
         <f t="shared" si="3"/>
-        <v>0.32688482632541138</v>
+        <v>32.688482632541138</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
@@ -2601,7 +2601,7 @@
       </c>
       <c r="E113" s="2">
         <f t="shared" si="3"/>
-        <v>0.46296175000000001</v>
+        <v>46.296174999999998</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
@@ -2620,7 +2620,7 @@
       </c>
       <c r="E114" s="2">
         <f t="shared" si="3"/>
-        <v>0.46633050000000004</v>
+        <v>46.633050000000004</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
@@ -2639,7 +2639,7 @@
       </c>
       <c r="E115" s="2">
         <f t="shared" si="3"/>
-        <v>3.1285499999999959E-2</v>
+        <v>3.1285499999999957</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
@@ -2658,7 +2658,7 @@
       </c>
       <c r="E116" s="2">
         <f t="shared" si="3"/>
-        <v>0.14824775000000009</v>
+        <v>14.82477500000001</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
@@ -2677,7 +2677,7 @@
       </c>
       <c r="E117" s="2">
         <f t="shared" si="3"/>
-        <v>0.44988125000000001</v>
+        <v>44.988125000000004</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
@@ -2696,7 +2696,7 @@
       </c>
       <c r="E118" s="2">
         <f t="shared" si="3"/>
-        <v>0.1317772499999999</v>
+        <v>13.17772499999999</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
@@ -2715,7 +2715,7 @@
       </c>
       <c r="E119" s="2">
         <f t="shared" si="3"/>
-        <v>0.46455350000000001</v>
+        <v>46.455350000000003</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
@@ -2734,7 +2734,7 @@
       </c>
       <c r="E120" s="2">
         <f t="shared" si="3"/>
-        <v>0.39702150000000003</v>
+        <v>39.702150000000003</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
@@ -2753,7 +2753,7 @@
       </c>
       <c r="E121" s="2">
         <f t="shared" si="3"/>
-        <v>0.56340849999999987</v>
+        <v>56.340849999999989</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
@@ -2772,7 +2772,7 @@
       </c>
       <c r="E122" s="2">
         <f t="shared" si="3"/>
-        <v>0.38054050000000006</v>
+        <v>38.054050000000004</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
@@ -2791,7 +2791,7 @@
       </c>
       <c r="E123" s="2">
         <f t="shared" si="3"/>
-        <v>0.13020175</v>
+        <v>13.020175</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
@@ -2810,7 +2810,7 @@
       </c>
       <c r="E124" s="2">
         <f t="shared" si="3"/>
-        <v>0.56507324999999997</v>
+        <v>56.507324999999994</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
@@ -2829,7 +2829,7 @@
       </c>
       <c r="E125" s="2">
         <f t="shared" si="3"/>
-        <v>0.36406149999999998</v>
+        <v>36.406149999999997</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
@@ -2848,7 +2848,7 @@
       </c>
       <c r="E126" s="2">
         <f t="shared" si="3"/>
-        <v>9.7221249999999967E-2</v>
+        <v>9.7221249999999966</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
@@ -2867,7 +2867,7 @@
       </c>
       <c r="E127" s="2">
         <f t="shared" si="3"/>
-        <v>0.59637350000000011</v>
+        <v>59.637350000000012</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
@@ -2886,7 +2886,7 @@
       </c>
       <c r="E128" s="2">
         <f t="shared" si="3"/>
-        <v>0.10351075000000001</v>
+        <v>10.351075000000002</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
@@ -2905,7 +2905,7 @@
       </c>
       <c r="E129" s="2">
         <f t="shared" si="3"/>
-        <v>0.33110925000000008</v>
+        <v>33.110925000000009</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
@@ -2924,7 +2924,7 @@
       </c>
       <c r="E130" s="2">
         <f t="shared" si="3"/>
-        <v>6.4248999999999973E-2</v>
+        <v>6.4248999999999974</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
@@ -2942,8 +2942,8 @@
         <v>-25776.630000000005</v>
       </c>
       <c r="E131" s="2">
-        <f t="shared" ref="E131:E143" si="5">IF(ISNUMBER(B131),ABS((C131-B131)/(B131)),"NAN")</f>
-        <v>0.64441575000000006</v>
+        <f t="shared" ref="E131:E143" si="5">IF(ISNUMBER(B131),ABS((C131-B131)/(B131))*100,"NAN")</f>
+        <v>64.441575</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
@@ -2962,7 +2962,7 @@
       </c>
       <c r="E132" s="2">
         <f t="shared" si="5"/>
-        <v>8.5648999999999975E-2</v>
+        <v>8.564899999999998</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
@@ -2981,7 +2981,7 @@
       </c>
       <c r="E133" s="2">
         <f t="shared" si="5"/>
-        <v>0.21779069767441864</v>
+        <v>21.779069767441865</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
@@ -3000,7 +3000,7 @@
       </c>
       <c r="E134" s="2">
         <f t="shared" si="5"/>
-        <v>9.9941860465116272E-2</v>
+        <v>9.9941860465116275</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
@@ -3019,7 +3019,7 @@
       </c>
       <c r="E135" s="2">
         <f t="shared" si="5"/>
-        <v>4.1744186046511665E-2</v>
+        <v>4.1744186046511667</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
@@ -3038,7 +3038,7 @@
       </c>
       <c r="E136" s="2">
         <f t="shared" si="5"/>
-        <v>2.136627906976751E-2</v>
+        <v>2.1366279069767509</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
@@ -3057,7 +3057,7 @@
       </c>
       <c r="E137" s="2">
         <f t="shared" si="5"/>
-        <v>7.5373831775700909E-2</v>
+        <v>7.5373831775700912</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
@@ -3076,7 +3076,7 @@
       </c>
       <c r="E138" s="2">
         <f t="shared" si="5"/>
-        <v>1.2336448598130777E-2</v>
+        <v>1.2336448598130778</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
@@ -3095,7 +3095,7 @@
       </c>
       <c r="E139" s="2">
         <f t="shared" si="5"/>
-        <v>4.3831775700934557E-2</v>
+        <v>4.3831775700934559</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
@@ -3114,7 +3114,7 @@
       </c>
       <c r="E140" s="2">
         <f t="shared" si="5"/>
-        <v>7.3504672897196213E-2</v>
+        <v>7.3504672897196217</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
@@ -3133,7 +3133,7 @@
       </c>
       <c r="E141" s="2">
         <f t="shared" si="5"/>
-        <v>7.3504672897196213E-2</v>
+        <v>7.3504672897196217</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
@@ -3152,7 +3152,7 @@
       </c>
       <c r="E142" s="2">
         <f t="shared" si="5"/>
-        <v>7.3504672897196213E-2</v>
+        <v>7.3504672897196217</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
@@ -3171,7 +3171,7 @@
       </c>
       <c r="E143" s="2">
         <f t="shared" si="5"/>
-        <v>1.0373831775700929E-2</v>
+        <v>1.0373831775700928</v>
       </c>
     </row>
   </sheetData>

</xml_diff>